<commit_message>
CIERRE  19 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/REMISIONES CENTRAL Dic-2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/REMISIONES CENTRAL Dic-2021.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL#14  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="VENTAS DIC 2021  " sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="VENTAS DE CENTRAL A ZAVALETA  " sheetId="4" r:id="rId4"/>
+    <sheet name="COMPRAS   OBRADOR   " sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3243" uniqueCount="92">
   <si>
     <t>Folio-Ticket</t>
   </si>
@@ -315,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +347,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +373,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF66CCFF"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -446,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -468,10 +489,42 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -8936,7 +8989,7 @@
   <dimension ref="A1:I279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17024,8 +17077,8 @@
   </sheetPr>
   <dimension ref="B1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F54" sqref="F53:F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17035,22 +17088,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="2:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
@@ -18214,4 +18267,2287 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:G126"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="19.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="24" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="23"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>803529</v>
+      </c>
+      <c r="B3" s="26">
+        <v>7898</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="28">
+        <v>2361.7800000000002</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>804274</v>
+      </c>
+      <c r="B4" s="26">
+        <v>7905</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="28">
+        <v>367.84</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>804311</v>
+      </c>
+      <c r="B5" s="32">
+        <v>7906</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="34">
+        <v>3023.02</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>804438</v>
+      </c>
+      <c r="B6" s="26">
+        <v>7908</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="28">
+        <v>174.36</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>804621</v>
+      </c>
+      <c r="B7" s="32">
+        <v>7910</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="34">
+        <v>5375</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>805013</v>
+      </c>
+      <c r="B8" s="32">
+        <v>7912</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="34">
+        <v>1920</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>805202</v>
+      </c>
+      <c r="B9" s="26">
+        <v>7913</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="28">
+        <v>9140</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>805455</v>
+      </c>
+      <c r="B10" s="32">
+        <v>7915</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="34">
+        <v>1017.52</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>805459</v>
+      </c>
+      <c r="B11" s="26">
+        <v>7916</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="28">
+        <v>107.42</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>805721</v>
+      </c>
+      <c r="B12" s="32">
+        <v>7917</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="34">
+        <v>140</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>805863</v>
+      </c>
+      <c r="B13" s="32">
+        <v>7919</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="34">
+        <v>4145.2</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>806067</v>
+      </c>
+      <c r="B14" s="26">
+        <v>7923</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="28">
+        <v>240</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
+        <v>806541</v>
+      </c>
+      <c r="B15" s="32">
+        <v>7924</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="34">
+        <v>422.4</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>806972</v>
+      </c>
+      <c r="B16" s="32">
+        <v>7929</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="34">
+        <v>550.79999999999995</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>807179</v>
+      </c>
+      <c r="B17" s="32">
+        <v>7931</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="34">
+        <v>10449.76</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="36"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>807268</v>
+      </c>
+      <c r="B18" s="32">
+        <v>7932</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="34">
+        <v>2256.92</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>807907</v>
+      </c>
+      <c r="B19" s="26">
+        <v>7935</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="28">
+        <v>654</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>808517</v>
+      </c>
+      <c r="B20" s="32">
+        <v>7937</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="34">
+        <v>87</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>808816</v>
+      </c>
+      <c r="B21" s="26">
+        <v>7940</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="28">
+        <v>270</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
+        <v>809934</v>
+      </c>
+      <c r="B22" s="32">
+        <v>7947</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="34">
+        <v>26018.6</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="36"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
+        <v>810096</v>
+      </c>
+      <c r="B23" s="32">
+        <v>7946</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="34">
+        <v>1232</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="36"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
+        <v>810472</v>
+      </c>
+      <c r="B24" s="32">
+        <v>7953</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="34">
+        <v>135.6</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="36"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>810484</v>
+      </c>
+      <c r="B25" s="26">
+        <v>7948</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="28">
+        <v>2574</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="30"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
+        <v>811409</v>
+      </c>
+      <c r="B26" s="26">
+        <v>7955</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="28">
+        <v>206.4</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="31">
+        <v>811512</v>
+      </c>
+      <c r="B27" s="32">
+        <v>7957</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="34">
+        <v>2214.8000000000002</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="36"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
+        <v>812213</v>
+      </c>
+      <c r="B28" s="32">
+        <v>7959</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="34">
+        <v>243</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="36"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
+        <v>812230</v>
+      </c>
+      <c r="B29" s="32">
+        <v>7960</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="34">
+        <v>4016</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="36"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
+        <v>812336</v>
+      </c>
+      <c r="B30" s="26">
+        <v>7962</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="28">
+        <v>15343.6</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>812886</v>
+      </c>
+      <c r="B31" s="32">
+        <v>7965</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="34">
+        <v>377.58</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="36"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="25">
+        <v>812887</v>
+      </c>
+      <c r="B32" s="26">
+        <v>7966</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="28">
+        <v>337.8</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
+        <v>813211</v>
+      </c>
+      <c r="B33" s="32">
+        <v>7967</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="34">
+        <v>1654</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="36"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="25">
+        <v>813275</v>
+      </c>
+      <c r="B34" s="26">
+        <v>7968</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="28">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
+        <v>814009</v>
+      </c>
+      <c r="B35" s="32">
+        <v>7969</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="34">
+        <v>113.4</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="36"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>814160</v>
+      </c>
+      <c r="B36" s="26">
+        <v>7970</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="28">
+        <v>242.4</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="25">
+        <v>814793</v>
+      </c>
+      <c r="B37" s="26">
+        <v>7976</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="28">
+        <v>8160.6</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="30"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="25">
+        <v>815340</v>
+      </c>
+      <c r="B38" s="26">
+        <v>7978</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="28">
+        <v>103.8</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="30"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="25">
+        <v>815631</v>
+      </c>
+      <c r="B39" s="26">
+        <v>7980</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="28">
+        <v>136.5</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="30"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="31">
+        <v>815745</v>
+      </c>
+      <c r="B40" s="32">
+        <v>7981</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="34">
+        <v>2226.06</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="36"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
+        <v>815923</v>
+      </c>
+      <c r="B41" s="32">
+        <v>7982</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="34">
+        <v>0</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="36"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="25">
+        <v>816090</v>
+      </c>
+      <c r="B42" s="26">
+        <v>7983</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="28">
+        <v>2446.44</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="30"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
+        <v>816139</v>
+      </c>
+      <c r="B43" s="32">
+        <v>7985</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="34">
+        <v>4342.3999999999996</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="36"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
+        <v>816730</v>
+      </c>
+      <c r="B44" s="26">
+        <v>7986</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="28">
+        <v>137.4</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="30"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <v>817233</v>
+      </c>
+      <c r="B45" s="26">
+        <v>7988</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="28">
+        <v>101.4</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="30"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="25">
+        <v>817419</v>
+      </c>
+      <c r="B46" s="26">
+        <v>7990</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="28">
+        <v>110.4</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="30"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="25">
+        <v>818680</v>
+      </c>
+      <c r="B47" s="26">
+        <v>7992</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="28">
+        <v>189.6</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="30"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="31">
+        <v>818681</v>
+      </c>
+      <c r="B48" s="32">
+        <v>7993</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="34">
+        <v>48.6</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="36"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="31">
+        <v>818710</v>
+      </c>
+      <c r="B49" s="32">
+        <v>7995</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="34">
+        <v>1901.2</v>
+      </c>
+      <c r="E49" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" s="36"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="31">
+        <v>818772</v>
+      </c>
+      <c r="B50" s="32">
+        <v>7997</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="34">
+        <v>1332.12</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" s="36"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="25">
+        <v>819187</v>
+      </c>
+      <c r="B51" s="26">
+        <v>8000</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="28">
+        <v>240</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="30"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="25">
+        <v>819430</v>
+      </c>
+      <c r="B52" s="26">
+        <v>8003</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="28">
+        <v>399.6</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="30"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="31">
+        <v>819651</v>
+      </c>
+      <c r="B53" s="32">
+        <v>8005</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="34">
+        <v>320.20999999999998</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="36"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="31">
+        <v>819696</v>
+      </c>
+      <c r="B54" s="32">
+        <v>8006</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="34">
+        <v>1584.68</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" s="36"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="25">
+        <v>819701</v>
+      </c>
+      <c r="B55" s="26">
+        <v>8007</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="28">
+        <v>309.60000000000002</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="30"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="31">
+        <v>819973</v>
+      </c>
+      <c r="B56" s="32">
+        <v>8010</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="34">
+        <v>870</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="36"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="31">
+        <v>820210</v>
+      </c>
+      <c r="B57" s="32">
+        <v>8013</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="34">
+        <v>336</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="36"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="25">
+        <v>820309</v>
+      </c>
+      <c r="B58" s="26">
+        <v>8014</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="28">
+        <v>642.4</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="30"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="31">
+        <v>820817</v>
+      </c>
+      <c r="B59" s="32">
+        <v>8015</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="34">
+        <v>107.1</v>
+      </c>
+      <c r="E59" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" s="36"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="25">
+        <v>820828</v>
+      </c>
+      <c r="B60" s="26">
+        <v>8017</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="28">
+        <v>17112</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="30"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="31">
+        <v>820831</v>
+      </c>
+      <c r="B61" s="32">
+        <v>8018</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="34">
+        <v>17372.400000000001</v>
+      </c>
+      <c r="E61" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61" s="36"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="25">
+        <v>820852</v>
+      </c>
+      <c r="B62" s="26">
+        <v>8016</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="28">
+        <v>14470.8</v>
+      </c>
+      <c r="E62" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="30"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="25">
+        <v>821318</v>
+      </c>
+      <c r="B63" s="26">
+        <v>8022</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="28">
+        <v>870</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F63" s="30"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="31">
+        <v>821357</v>
+      </c>
+      <c r="B64" s="32">
+        <v>8023</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="34">
+        <v>1098.24</v>
+      </c>
+      <c r="E64" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="36"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="31">
+        <v>821910</v>
+      </c>
+      <c r="B65" s="32">
+        <v>8026</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="34">
+        <v>2012</v>
+      </c>
+      <c r="E65" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="36"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="31">
+        <v>821949</v>
+      </c>
+      <c r="B66" s="32">
+        <v>8025</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="34">
+        <v>1284.8</v>
+      </c>
+      <c r="E66" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="36"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="31">
+        <v>822186</v>
+      </c>
+      <c r="B67" s="32">
+        <v>8029</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="34">
+        <v>2169.6</v>
+      </c>
+      <c r="E67" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="36"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="25">
+        <v>822341</v>
+      </c>
+      <c r="B68" s="26">
+        <v>8030</v>
+      </c>
+      <c r="C68" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="28">
+        <v>297</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="30"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="31">
+        <v>823119</v>
+      </c>
+      <c r="B69" s="32">
+        <v>8035</v>
+      </c>
+      <c r="C69" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" s="34">
+        <v>54.6</v>
+      </c>
+      <c r="E69" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="36"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="25">
+        <v>823128</v>
+      </c>
+      <c r="B70" s="26">
+        <v>8036</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" s="28">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="30"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="31">
+        <v>823377</v>
+      </c>
+      <c r="B71" s="32">
+        <v>8045</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="34">
+        <v>1044</v>
+      </c>
+      <c r="E71" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" s="36"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="25">
+        <v>824567</v>
+      </c>
+      <c r="B72" s="26">
+        <v>8048</v>
+      </c>
+      <c r="C72" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="28">
+        <v>429</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="30"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="31">
+        <v>824582</v>
+      </c>
+      <c r="B73" s="32">
+        <v>8049</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="34">
+        <v>12206</v>
+      </c>
+      <c r="E73" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" s="36"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="31">
+        <v>824748</v>
+      </c>
+      <c r="B74" s="32">
+        <v>8051</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" s="34">
+        <v>6984</v>
+      </c>
+      <c r="E74" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" s="36"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="31">
+        <v>825962</v>
+      </c>
+      <c r="B75" s="32">
+        <v>8057</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" s="34">
+        <v>244.8</v>
+      </c>
+      <c r="E75" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="36"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="25">
+        <v>826036</v>
+      </c>
+      <c r="B76" s="26">
+        <v>8058</v>
+      </c>
+      <c r="C76" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="28">
+        <v>96</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F76" s="30"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="25">
+        <v>827607</v>
+      </c>
+      <c r="B77" s="26">
+        <v>8062</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="28">
+        <v>331.5</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F77" s="30"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="31">
+        <v>827658</v>
+      </c>
+      <c r="B78" s="32">
+        <v>8063</v>
+      </c>
+      <c r="C78" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D78" s="34">
+        <v>2385.7600000000002</v>
+      </c>
+      <c r="E78" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F78" s="36"/>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="31">
+        <v>827688</v>
+      </c>
+      <c r="B79" s="32">
+        <v>8064</v>
+      </c>
+      <c r="C79" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" s="34">
+        <v>110</v>
+      </c>
+      <c r="E79" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" s="36"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="25">
+        <v>827731</v>
+      </c>
+      <c r="B80" s="26">
+        <v>8066</v>
+      </c>
+      <c r="C80" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" s="28">
+        <v>11814.4</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F80" s="30"/>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="31">
+        <v>827855</v>
+      </c>
+      <c r="B81" s="32">
+        <v>8069</v>
+      </c>
+      <c r="C81" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81" s="34">
+        <v>405.6</v>
+      </c>
+      <c r="E81" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F81" s="36"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="25">
+        <v>827955</v>
+      </c>
+      <c r="B82" s="26">
+        <v>8070</v>
+      </c>
+      <c r="C82" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" s="28">
+        <v>4824</v>
+      </c>
+      <c r="E82" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="30"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="25">
+        <v>828799</v>
+      </c>
+      <c r="B83" s="26">
+        <v>8074</v>
+      </c>
+      <c r="C83" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D83" s="28">
+        <v>512</v>
+      </c>
+      <c r="E83" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" s="30"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="31">
+        <v>828978</v>
+      </c>
+      <c r="B84" s="32">
+        <v>8075</v>
+      </c>
+      <c r="C84" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="34">
+        <v>512</v>
+      </c>
+      <c r="E84" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" s="36"/>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="25">
+        <v>828984</v>
+      </c>
+      <c r="B85" s="26">
+        <v>8076</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" s="28">
+        <v>454.5</v>
+      </c>
+      <c r="E85" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" s="30"/>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="25">
+        <v>829006</v>
+      </c>
+      <c r="B86" s="26">
+        <v>8078</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86" s="28">
+        <v>2480.56</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F86" s="30"/>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="25">
+        <v>829051</v>
+      </c>
+      <c r="B87" s="26">
+        <v>8079</v>
+      </c>
+      <c r="C87" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="28">
+        <v>348</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" s="30"/>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="25">
+        <v>829098</v>
+      </c>
+      <c r="B88" s="26">
+        <v>8081</v>
+      </c>
+      <c r="C88" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" s="28">
+        <v>1020</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F88" s="30"/>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="31">
+        <v>830408</v>
+      </c>
+      <c r="B89" s="32">
+        <v>8093</v>
+      </c>
+      <c r="C89" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="34">
+        <v>486</v>
+      </c>
+      <c r="E89" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F89" s="36"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="25">
+        <v>830582</v>
+      </c>
+      <c r="B90" s="26">
+        <v>8094</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D90" s="28">
+        <v>1647</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F90" s="30"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="25">
+        <v>832228</v>
+      </c>
+      <c r="B91" s="26">
+        <v>8098</v>
+      </c>
+      <c r="C91" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91" s="28">
+        <v>380.4</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F91" s="30"/>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="25">
+        <v>832286</v>
+      </c>
+      <c r="B92" s="26">
+        <v>8100</v>
+      </c>
+      <c r="C92" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" s="28">
+        <v>0</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F92" s="30"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="31">
+        <v>832294</v>
+      </c>
+      <c r="B93" s="32">
+        <v>8103</v>
+      </c>
+      <c r="C93" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" s="34">
+        <v>1234.8</v>
+      </c>
+      <c r="E93" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F93" s="36"/>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="25">
+        <v>833327</v>
+      </c>
+      <c r="B94" s="26">
+        <v>8106</v>
+      </c>
+      <c r="C94" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="28">
+        <v>82.5</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F94" s="30"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="31">
+        <v>833472</v>
+      </c>
+      <c r="B95" s="32">
+        <v>8107</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="34">
+        <v>528.96</v>
+      </c>
+      <c r="E95" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F95" s="36"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="25">
+        <v>833535</v>
+      </c>
+      <c r="B96" s="26">
+        <v>8108</v>
+      </c>
+      <c r="C96" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D96" s="28">
+        <v>1485.32</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F96" s="30"/>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="31">
+        <v>834310</v>
+      </c>
+      <c r="B97" s="32">
+        <v>8113</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D97" s="34">
+        <v>93</v>
+      </c>
+      <c r="E97" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F97" s="36"/>
+    </row>
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="25">
+        <v>834635</v>
+      </c>
+      <c r="B98" s="26">
+        <v>8116</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D98" s="28">
+        <v>494.28</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F98" s="30"/>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="31">
+        <v>835413</v>
+      </c>
+      <c r="B99" s="32">
+        <v>8117</v>
+      </c>
+      <c r="C99" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="34">
+        <v>1397.22</v>
+      </c>
+      <c r="E99" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F99" s="36"/>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="25">
+        <v>836021</v>
+      </c>
+      <c r="B100" s="26">
+        <v>8118</v>
+      </c>
+      <c r="C100" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="28">
+        <v>570.08000000000004</v>
+      </c>
+      <c r="E100" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F100" s="30"/>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="31">
+        <v>836100</v>
+      </c>
+      <c r="B101" s="32">
+        <v>8119</v>
+      </c>
+      <c r="C101" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D101" s="34">
+        <v>295.8</v>
+      </c>
+      <c r="E101" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F101" s="36"/>
+    </row>
+    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="25">
+        <v>836372</v>
+      </c>
+      <c r="B102" s="26">
+        <v>8120</v>
+      </c>
+      <c r="C102" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" s="28">
+        <v>535.96</v>
+      </c>
+      <c r="E102" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F102" s="30"/>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="25">
+        <v>836668</v>
+      </c>
+      <c r="B103" s="26">
+        <v>8122</v>
+      </c>
+      <c r="C103" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D103" s="28">
+        <v>744</v>
+      </c>
+      <c r="E103" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F103" s="30"/>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="25">
+        <v>837367</v>
+      </c>
+      <c r="B104" s="26">
+        <v>8126</v>
+      </c>
+      <c r="C104" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" s="28">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E104" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F104" s="30"/>
+    </row>
+    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="31">
+        <v>837450</v>
+      </c>
+      <c r="B105" s="32">
+        <v>8128</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D105" s="34">
+        <v>7218</v>
+      </c>
+      <c r="E105" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F105" s="36"/>
+    </row>
+    <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="25">
+        <v>837489</v>
+      </c>
+      <c r="B106" s="26">
+        <v>8127</v>
+      </c>
+      <c r="C106" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D106" s="28">
+        <v>11627.2</v>
+      </c>
+      <c r="E106" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F106" s="30"/>
+    </row>
+    <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="25">
+        <v>837960</v>
+      </c>
+      <c r="B107" s="26">
+        <v>8130</v>
+      </c>
+      <c r="C107" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D107" s="28">
+        <v>216</v>
+      </c>
+      <c r="E107" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F107" s="30"/>
+    </row>
+    <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="31">
+        <v>838387</v>
+      </c>
+      <c r="B108" s="32">
+        <v>8131</v>
+      </c>
+      <c r="C108" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D108" s="34">
+        <v>133.80000000000001</v>
+      </c>
+      <c r="E108" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F108" s="36"/>
+    </row>
+    <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="25">
+        <v>838426</v>
+      </c>
+      <c r="B109" s="26">
+        <v>8134</v>
+      </c>
+      <c r="C109" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D109" s="28">
+        <v>2929.66</v>
+      </c>
+      <c r="E109" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F109" s="30"/>
+    </row>
+    <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="31">
+        <v>838689</v>
+      </c>
+      <c r="B110" s="32">
+        <v>8135</v>
+      </c>
+      <c r="C110" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D110" s="34">
+        <v>878.7</v>
+      </c>
+      <c r="E110" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F110" s="36"/>
+    </row>
+    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="25">
+        <v>838691</v>
+      </c>
+      <c r="B111" s="26">
+        <v>8136</v>
+      </c>
+      <c r="C111" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D111" s="28">
+        <v>561.05999999999995</v>
+      </c>
+      <c r="E111" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F111" s="30"/>
+    </row>
+    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="25">
+        <v>839385</v>
+      </c>
+      <c r="B112" s="26">
+        <v>8139</v>
+      </c>
+      <c r="C112" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D112" s="28">
+        <v>243</v>
+      </c>
+      <c r="E112" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F112" s="30"/>
+    </row>
+    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="31">
+        <v>839563</v>
+      </c>
+      <c r="B113" s="32">
+        <v>8141</v>
+      </c>
+      <c r="C113" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D113" s="34">
+        <v>13086</v>
+      </c>
+      <c r="E113" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F113" s="36"/>
+    </row>
+    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="25">
+        <v>839568</v>
+      </c>
+      <c r="B114" s="26">
+        <v>8142</v>
+      </c>
+      <c r="C114" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D114" s="28">
+        <v>112.8</v>
+      </c>
+      <c r="E114" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F114" s="30"/>
+    </row>
+    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="25">
+        <v>839632</v>
+      </c>
+      <c r="B115" s="26">
+        <v>8143</v>
+      </c>
+      <c r="C115" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D115" s="28">
+        <v>411.7</v>
+      </c>
+      <c r="E115" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F115" s="30"/>
+    </row>
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="31">
+        <v>840924</v>
+      </c>
+      <c r="B116" s="32">
+        <v>8149</v>
+      </c>
+      <c r="C116" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D116" s="34">
+        <v>70.2</v>
+      </c>
+      <c r="E116" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" s="36"/>
+    </row>
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="25">
+        <v>842194</v>
+      </c>
+      <c r="B117" s="26">
+        <v>8156</v>
+      </c>
+      <c r="C117" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D117" s="28">
+        <v>297.60000000000002</v>
+      </c>
+      <c r="E117" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F117" s="30"/>
+    </row>
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="25">
+        <v>842569</v>
+      </c>
+      <c r="B118" s="26">
+        <v>8158</v>
+      </c>
+      <c r="C118" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D118" s="28">
+        <v>2962.38</v>
+      </c>
+      <c r="E118" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F118" s="30"/>
+    </row>
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="31">
+        <v>842724</v>
+      </c>
+      <c r="B119" s="32">
+        <v>8159</v>
+      </c>
+      <c r="C119" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119" s="34">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="E119" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F119" s="36"/>
+    </row>
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="25">
+        <v>842800</v>
+      </c>
+      <c r="B120" s="26">
+        <v>8160</v>
+      </c>
+      <c r="C120" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D120" s="28">
+        <v>4368</v>
+      </c>
+      <c r="E120" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F120" s="30"/>
+    </row>
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="25">
+        <v>843183</v>
+      </c>
+      <c r="B121" s="26">
+        <v>8162</v>
+      </c>
+      <c r="C121" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D121" s="28">
+        <v>6552</v>
+      </c>
+      <c r="E121" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F121" s="30"/>
+    </row>
+    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="25">
+        <v>843213</v>
+      </c>
+      <c r="B122" s="26">
+        <v>8163</v>
+      </c>
+      <c r="C122" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D122" s="28">
+        <v>6318</v>
+      </c>
+      <c r="E122" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F122" s="30"/>
+    </row>
+    <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="31">
+        <v>843337</v>
+      </c>
+      <c r="B123" s="32">
+        <v>8165</v>
+      </c>
+      <c r="C123" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D123" s="34">
+        <v>2164.86</v>
+      </c>
+      <c r="E123" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F123" s="36"/>
+    </row>
+    <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A124" s="25">
+        <v>843473</v>
+      </c>
+      <c r="B124" s="26">
+        <v>8166</v>
+      </c>
+      <c r="C124" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D124" s="28">
+        <v>587.4</v>
+      </c>
+      <c r="E124" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F124" s="30"/>
+    </row>
+    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="25">
+        <v>845036</v>
+      </c>
+      <c r="B125" s="26">
+        <v>8168</v>
+      </c>
+      <c r="C125" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D125" s="28">
+        <v>537</v>
+      </c>
+      <c r="E125" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F125" s="30"/>
+    </row>
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="31">
+        <v>846142</v>
+      </c>
+      <c r="B126" s="32">
+        <v>8174</v>
+      </c>
+      <c r="C126" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D126" s="34">
+        <v>1081.2</v>
+      </c>
+      <c r="E126" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F126" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>